<commit_message>
Modified some changes in the CSS
Modified some changes in the CSS
</commit_message>
<xml_diff>
--- a/Input/Temp_balanced_DPT_scen2.xlsx
+++ b/Input/Temp_balanced_DPT_scen2.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C790"/>
+  <dimension ref="A1:C792"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12301,6 +12301,24 @@
         </is>
       </c>
       <c r="C790" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr"/>
+      <c r="B791" t="inlineStr"/>
+      <c r="C791" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr"/>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="C792" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12315,7 +12333,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D790"/>
+  <dimension ref="A1:D792"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26544,6 +26562,30 @@
         <v>0</v>
       </c>
       <c r="D790" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr"/>
+      <c r="B791" t="inlineStr"/>
+      <c r="C791" t="n">
+        <v>0</v>
+      </c>
+      <c r="D791" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr"/>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="C792" t="n">
+        <v>0</v>
+      </c>
+      <c r="D792" t="n">
         <v>0</v>
       </c>
     </row>
@@ -26558,7 +26600,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C790"/>
+  <dimension ref="A1:C792"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38415,6 +38457,24 @@
         </is>
       </c>
       <c r="C790" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr"/>
+      <c r="B791" t="inlineStr"/>
+      <c r="C791" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr"/>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="C792" t="n">
         <v>0</v>
       </c>
     </row>
@@ -38429,7 +38489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D790"/>
+  <dimension ref="A1:D792"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52658,6 +52718,30 @@
         <v>0</v>
       </c>
       <c r="D790" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr"/>
+      <c r="B791" t="inlineStr"/>
+      <c r="C791" t="n">
+        <v>0</v>
+      </c>
+      <c r="D791" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr"/>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="C792" t="n">
+        <v>0</v>
+      </c>
+      <c r="D792" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>